<commit_message>
add mcu, crystal, and programming header to schematic
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -143,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -244,13 +244,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -632,11 +632,11 @@
         <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>4.33</v>
+        <v>7.78</v>
       </c>
       <c r="J3" s="6">
         <f>I3*H3</f>
-        <v>4.33</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J37" si="0">I4*H4</f>
+        <f t="shared" ref="J4:J11" si="0">I4*H4</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="K4" t="s">
@@ -804,7 +804,7 @@
       </c>
       <c r="J20" s="11">
         <f>SUM(J3:J11)</f>
-        <v>43.564</v>
+        <v>47.013999999999996</v>
       </c>
     </row>
     <row r="21" spans="9:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
create initial panel artwork design and update the BOM with some mechanical items.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,8 +15,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>paul musgrave</author>
+  </authors>
+  <commentList>
+    <comment ref="D21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>paul musgrave:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aliexpress has a lot of potential, just have to shop around for specifics. Putting in $0.50/pc as a placeholder.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>paul musgrave:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+these are the wrong switches for some of them. They'll work for the envelope_bypass though.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -136,6 +194,60 @@
   </si>
   <si>
     <t>SUBTOTAL:</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Chassis - Steel 7" x 5" x 2"</t>
+  </si>
+  <si>
+    <t>Hammond</t>
+  </si>
+  <si>
+    <t>1441-12BK3</t>
+  </si>
+  <si>
+    <t>546-1441-12BK3</t>
+  </si>
+  <si>
+    <t>Bottom Plate 7 x 5" 20AWG Steel Black</t>
+  </si>
+  <si>
+    <t>1431-12BK3</t>
+  </si>
+  <si>
+    <t>546-1431-12BK3</t>
+  </si>
+  <si>
+    <t>Toggle Switches SPST ON-OFF STD LVR</t>
+  </si>
+  <si>
+    <t>Knobs</t>
+  </si>
+  <si>
+    <t>Toggle Switches SPDT ON-ON</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>PCB, Control Board</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>PCB, Main Synth Board</t>
   </si>
 </sst>
 </file>
@@ -145,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +293,19 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -554,28 +679,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,27 +723,30 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -628,18 +759,21 @@
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="8">
+      <c r="G3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="8">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
-        <v>7.78</v>
-      </c>
       <c r="J3" s="6">
-        <f>I3*H3</f>
-        <v>7.78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.23</v>
+      </c>
+      <c r="K3" s="6">
+        <f>J3*I3</f>
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -652,21 +786,24 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="8">
+      <c r="G4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="8">
         <v>2</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J4" s="6">
-        <f t="shared" ref="J4:J11" si="0">I4*H4</f>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K25" si="0">J4*I4</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -679,21 +816,24 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8">
+      <c r="G5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="8">
         <v>1</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>0.59</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>17</v>
       </c>
@@ -706,21 +846,24 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="8">
+      <c r="G6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="8">
         <v>8</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>0.4</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -733,39 +876,42 @@
       <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="8">
+      <c r="G7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="8">
         <v>8</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <v>0.4</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J8" s="6">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J9" s="6">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -781,36 +927,296 @@
       <c r="F11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <v>48</v>
       </c>
-      <c r="I11" s="9">
+      <c r="J11" s="9">
         <v>0.64800000000000002</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <f t="shared" si="0"/>
         <v>31.103999999999999</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="10" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="6">
+        <f>J12*I12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <v>13.24</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="0"/>
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>4.82</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="0"/>
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="8">
+        <v>27</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="8">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="8">
+        <v>9</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="8">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6">
+        <v>2</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="8">
+        <v>1</v>
+      </c>
+      <c r="J25" s="6">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="11">
-        <f>SUM(J3:J11)</f>
-        <v>47.013999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="9:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="K27" s="11">
+        <f>SUM(K3:K25)</f>
+        <v>86.703999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update BOM with new switch and knob prices from Aliexpress
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -21,7 +21,7 @@
     <author>paul musgrave</author>
   </authors>
   <commentList>
-    <comment ref="D21" authorId="0">
+    <comment ref="D22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Item</t>
   </si>
@@ -223,9 +223,6 @@
     <t>546-1431-12BK3</t>
   </si>
   <si>
-    <t>Toggle Switches SPST ON-OFF STD LVR</t>
-  </si>
-  <si>
     <t>Knobs</t>
   </si>
   <si>
@@ -248,6 +245,18 @@
   </si>
   <si>
     <t>PCB, Main Synth Board</t>
+  </si>
+  <si>
+    <t>Enclosures, Boxes, &amp; Cases Diecast Alum Black 7.38 x 7.38 x 2.48"</t>
+  </si>
+  <si>
+    <t>1590FBK</t>
+  </si>
+  <si>
+    <t>546-1590F-BK</t>
+  </si>
+  <si>
+    <t>Toggle Switches SPST ON-OFF-ON</t>
   </si>
 </sst>
 </file>
@@ -257,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +315,21 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -361,7 +385,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -376,6 +400,12 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -680,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -760,7 +790,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="8">
         <v>1</v>
@@ -787,7 +817,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="8">
         <v>2</v>
@@ -796,7 +826,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" ref="K4:K25" si="0">J4*I4</f>
+        <f t="shared" ref="K4:K26" si="0">J4*I4</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="L4" t="s">
@@ -817,7 +847,7 @@
         <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" s="8">
         <v>1</v>
@@ -847,7 +877,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="8">
         <v>8</v>
@@ -877,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="8">
         <v>8</v>
@@ -928,20 +958,20 @@
         <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I11" s="8">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J11" s="9">
         <v>0.64800000000000002</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="0"/>
-        <v>31.103999999999999</v>
+        <v>17.496000000000002</v>
       </c>
       <c r="L11" t="s">
         <v>36</v>
@@ -993,95 +1023,105 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>45</v>
       </c>
       <c r="I19" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="6">
         <v>13.24</v>
       </c>
       <c r="K19" s="6">
         <f t="shared" si="0"/>
-        <v>13.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>48</v>
       </c>
       <c r="I20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="6">
         <v>4.82</v>
       </c>
       <c r="K20" s="6">
         <f t="shared" si="0"/>
-        <v>4.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="I21" s="8">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="J21" s="6">
-        <v>0.5</v>
+        <v>31.15</v>
       </c>
       <c r="K21" s="6">
         <f t="shared" si="0"/>
-        <v>13.5</v>
+        <v>31.15</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1094,21 +1134,20 @@
       <c r="D22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="8">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="J22" s="6">
-        <v>0.22</v>
+        <v>0.39</v>
       </c>
       <c r="K22" s="6">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>10.530000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1119,23 +1158,23 @@
         <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="8">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J23" s="6">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="K23" s="6">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1146,25 +1185,23 @@
         <v>41</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J24" s="6">
-        <v>2</v>
+        <v>0.19</v>
       </c>
       <c r="K24" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1175,44 +1212,73 @@
         <v>41</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="8">
         <v>1</v>
       </c>
       <c r="J25" s="6">
+        <v>2</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="8">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
         <v>5</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K26" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="11">
-        <f>SUM(K3:K25)</f>
-        <v>86.703999999999994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="K28" s="11">
+        <f>SUM(K3:K26)</f>
+        <v>82.016000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>